<commit_message>
[Maintain_Job_Status] : Test Data Added
</commit_message>
<xml_diff>
--- a/TestData/MaintainJobSt.xlsx
+++ b/TestData/MaintainJobSt.xlsx
@@ -121,22 +121,22 @@
     <t>AAA</t>
   </si>
   <si>
-    <t>03</t>
-  </si>
-  <si>
     <t>Update Status</t>
   </si>
   <si>
-    <t>11-Jul-2023</t>
-  </si>
-  <si>
-    <t>12-Jul-2023</t>
-  </si>
-  <si>
-    <t>59</t>
-  </si>
-  <si>
-    <t>CHN/BKG/AFE/00184/23-24</t>
+    <t>CHN/BKG/AFE/00195/23-24</t>
+  </si>
+  <si>
+    <t>10-Jul-2023</t>
+  </si>
+  <si>
+    <t>14-Jul-2023</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>06</t>
   </si>
 </sst>
 </file>
@@ -500,6 +500,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="15" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -510,12 +516,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="15" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -801,8 +801,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -859,11 +859,11 @@
       <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="17"/>
-      <c r="D3" s="18"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="20"/>
     </row>
     <row r="4" spans="1:10" ht="21" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
@@ -914,10 +914,10 @@
       <c r="E7" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="19" t="s">
+      <c r="F7" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="G7" s="19"/>
+      <c r="G7" s="21"/>
       <c r="H7" s="9" t="s">
         <v>12</v>
       </c>
@@ -936,7 +936,7 @@
         <v>1</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D8" s="10" t="s">
         <v>13</v>
@@ -944,17 +944,17 @@
       <c r="E8" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="F8" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="G8" s="21" t="s">
+      <c r="F8" s="16" t="s">
         <v>21</v>
+      </c>
+      <c r="G8" s="17" t="s">
+        <v>22</v>
       </c>
       <c r="H8" s="10" t="s">
         <v>16</v>
       </c>
       <c r="I8" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J8" s="14" t="s">
         <v>20</v>

</xml_diff>